<commit_message>
notthing new hope so
</commit_message>
<xml_diff>
--- a/file/btc_weekly_return.xlsx
+++ b/file/btc_weekly_return.xlsx
@@ -385,7 +385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G374"/>
+  <dimension ref="A1:G376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8976,15 +8976,61 @@
         <v>44550</v>
       </c>
       <c r="D374" t="n">
-        <v>46688.4</v>
+        <v>46687.19</v>
       </c>
       <c r="E374" t="n">
+        <v>50792.036921</v>
+      </c>
+      <c r="F374" t="n">
+        <v>-0.06816445630582346</v>
+      </c>
+      <c r="G374" t="n">
+        <v>0.08789414332039636</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7">
+      <c r="A375" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B375" t="n">
+        <v>373</v>
+      </c>
+      <c r="C375" s="2" t="n">
+        <v>44557</v>
+      </c>
+      <c r="D375" t="n">
+        <v>50792.240989</v>
+      </c>
+      <c r="E375" t="n">
+        <v>47317.947964</v>
+      </c>
+      <c r="F375" t="n">
+        <v>0.08792670942500491</v>
+      </c>
+      <c r="G375" t="n">
+        <v>-0.0683982995681679</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7">
+      <c r="A376" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B376" t="n">
+        <v>374</v>
+      </c>
+      <c r="C376" s="2" t="n">
+        <v>44564</v>
+      </c>
+      <c r="D376" t="n">
+        <v>47316.178587</v>
+      </c>
+      <c r="E376" t="n">
         <v>0</v>
       </c>
-      <c r="F374" t="n">
-        <v>-0.06814030576243302</v>
-      </c>
-      <c r="G374" t="n">
+      <c r="F376" t="n">
+        <v>-0.0684368780411323</v>
+      </c>
+      <c r="G376" t="n">
         <v>-1</v>
       </c>
     </row>

</xml_diff>